<commit_message>
Update incoming orders spreadsheet
Replace binary Excel file data/incoming_orders_data.xlsx with an updated version containing refreshed incoming orders data. The diff is binary, so contents are not shown here.
</commit_message>
<xml_diff>
--- a/data/incoming_orders_data.xlsx
+++ b/data/incoming_orders_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Project Files\Daily Python\Day11\flaskProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\DesktopFiles\Cupstock\shuangshuangstore\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2523C1-C0D0-43D0-8E2D-FFD107730637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D03D240-F74E-4F51-9DB0-E028FC133EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5510" yWindow="1180" windowWidth="30780" windowHeight="19700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1770" yWindow="840" windowWidth="33730" windowHeight="19700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="276">
   <si>
     <t>source</t>
   </si>
@@ -49,9 +49,6 @@
     <t>LoveShackFancy</t>
   </si>
   <si>
-    <t>Stanley1913-CJ</t>
-  </si>
-  <si>
     <t>#12115388</t>
   </si>
   <si>
@@ -368,9 +365,6 @@
   </si>
   <si>
     <t>——</t>
-  </si>
-  <si>
-    <t>Stanley1914</t>
   </si>
   <si>
     <t>#12155073</t>
@@ -1294,8 +1288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="E106" sqref="E106"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56:A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1337,22 +1331,22 @@
         <v>8</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -1360,22 +1354,22 @@
         <v>8</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -1383,22 +1377,22 @@
         <v>8</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -1406,22 +1400,22 @@
         <v>8</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -1429,22 +1423,22 @@
         <v>8</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -1452,22 +1446,22 @@
         <v>8</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -1475,22 +1469,22 @@
         <v>8</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -1498,22 +1492,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -1521,22 +1515,22 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -1544,22 +1538,22 @@
         <v>7</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -1567,22 +1561,22 @@
         <v>7</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -1590,22 +1584,22 @@
         <v>7</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="F13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -1613,22 +1607,22 @@
         <v>7</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="F14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -1636,22 +1630,22 @@
         <v>7</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -1659,22 +1653,22 @@
         <v>7</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -1682,22 +1676,22 @@
         <v>7</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -1705,22 +1699,22 @@
         <v>7</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -1728,22 +1722,22 @@
         <v>7</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -1751,22 +1745,22 @@
         <v>7</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -1774,22 +1768,22 @@
         <v>7</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>33</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -1797,22 +1791,22 @@
         <v>7</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -1820,22 +1814,22 @@
         <v>7</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -1843,22 +1837,22 @@
         <v>7</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -1866,22 +1860,22 @@
         <v>7</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
@@ -1889,22 +1883,22 @@
         <v>7</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -1912,22 +1906,22 @@
         <v>7</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
@@ -1935,22 +1929,22 @@
         <v>7</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
@@ -1958,22 +1952,22 @@
         <v>7</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
@@ -1981,22 +1975,22 @@
         <v>7</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
@@ -2004,22 +1998,22 @@
         <v>7</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
@@ -2027,22 +2021,22 @@
         <v>7</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
@@ -2050,45 +2044,45 @@
         <v>7</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D33" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>122</v>
-      </c>
       <c r="F33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>116</v>
+        <v>7</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D34" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="F34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
@@ -2096,482 +2090,482 @@
         <v>7</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F37" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C39" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F39" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F41" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F43" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C44" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F44" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C46" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F46" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C47" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F48" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C49" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F49" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F50" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C51" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F51" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C52" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C53" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F53" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C54" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F54" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C55" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F55" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
@@ -2579,22 +2573,22 @@
         <v>7</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C56" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F56" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
@@ -2602,22 +2596,22 @@
         <v>7</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C57" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
@@ -2625,22 +2619,22 @@
         <v>7</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C58" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
@@ -2648,22 +2642,22 @@
         <v>7</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C59" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F59" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
@@ -2671,22 +2665,22 @@
         <v>7</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C60" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F60" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
@@ -2694,45 +2688,45 @@
         <v>7</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C61" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F61" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>116</v>
+        <v>7</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C62" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F62" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
@@ -2740,22 +2734,22 @@
         <v>7</v>
       </c>
       <c r="B63" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D63" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="C63" t="s">
-        <v>32</v>
-      </c>
-      <c r="D63" s="11" t="s">
-        <v>165</v>
-      </c>
       <c r="E63" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F63" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
@@ -2763,22 +2757,22 @@
         <v>7</v>
       </c>
       <c r="B64" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C64" t="s">
-        <v>32</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="F64" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
@@ -2786,22 +2780,22 @@
         <v>8</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C65" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D65" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="E65" s="2" t="s">
-        <v>176</v>
-      </c>
       <c r="F65" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
@@ -2809,22 +2803,22 @@
         <v>8</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C66" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D66" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="E66" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E66" s="2" t="s">
-        <v>177</v>
-      </c>
       <c r="F66" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
@@ -2832,22 +2826,22 @@
         <v>8</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C67" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F67" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
@@ -2855,22 +2849,22 @@
         <v>8</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C68" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F68" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
@@ -2878,22 +2872,22 @@
         <v>7</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C69" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F69" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
@@ -2901,206 +2895,206 @@
         <v>7</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C70" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F70" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B71" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C71" t="s">
+        <v>31</v>
+      </c>
+      <c r="D71" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="C71" t="s">
-        <v>32</v>
-      </c>
-      <c r="D71" s="9" t="s">
-        <v>184</v>
-      </c>
       <c r="E71" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F71" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
+        <v>179</v>
+      </c>
+      <c r="B72" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="B72" s="4" t="s">
-        <v>183</v>
-      </c>
       <c r="C72" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F72" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C73" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F73" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C74" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F74" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C75" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F75" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B76" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="C76" t="s">
+        <v>31</v>
+      </c>
+      <c r="D76" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="C76" t="s">
-        <v>32</v>
-      </c>
-      <c r="D76" s="9" t="s">
-        <v>199</v>
-      </c>
       <c r="E76" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F76" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B77" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="C77" t="s">
+        <v>31</v>
+      </c>
+      <c r="D77" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C77" t="s">
-        <v>32</v>
-      </c>
-      <c r="D77" s="9" t="s">
-        <v>202</v>
-      </c>
       <c r="E77" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F77" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B78" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="C78" t="s">
+        <v>31</v>
+      </c>
+      <c r="D78" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="C78" t="s">
-        <v>32</v>
-      </c>
-      <c r="D78" s="9" t="s">
-        <v>203</v>
-      </c>
       <c r="E78" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F78" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
@@ -3108,22 +3102,22 @@
         <v>7</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C79" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F79" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
@@ -3131,22 +3125,22 @@
         <v>7</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C80" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F80" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
@@ -3154,22 +3148,22 @@
         <v>7</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C81" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F81" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
@@ -3177,22 +3171,22 @@
         <v>7</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C82" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F82" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
@@ -3200,22 +3194,22 @@
         <v>7</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C83" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F83" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
@@ -3223,22 +3217,22 @@
         <v>7</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C84" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F84" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
@@ -3246,22 +3240,22 @@
         <v>7</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C85" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D85" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F85" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G85" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
@@ -3269,114 +3263,114 @@
         <v>7</v>
       </c>
       <c r="B86" t="s">
+        <v>228</v>
+      </c>
+      <c r="C86" t="s">
+        <v>31</v>
+      </c>
+      <c r="D86" t="s">
+        <v>229</v>
+      </c>
+      <c r="E86" t="s">
         <v>230</v>
       </c>
-      <c r="C86" t="s">
-        <v>32</v>
-      </c>
-      <c r="D86" t="s">
-        <v>231</v>
-      </c>
-      <c r="E86" t="s">
-        <v>232</v>
-      </c>
       <c r="F86" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G86" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B87" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C87" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D87" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E87" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F87" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B88" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C88" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D88" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E88" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F88" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G88" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B89" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C89" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D89" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E89" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F89" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G89" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B90" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C90" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D90" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E90" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F90" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G90" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
@@ -3384,22 +3378,22 @@
         <v>8</v>
       </c>
       <c r="B91" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C91" t="s">
+        <v>31</v>
+      </c>
+      <c r="D91" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="E91" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="C91" t="s">
-        <v>32</v>
-      </c>
-      <c r="D91" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>277</v>
-      </c>
       <c r="F91" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G91" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.35">
@@ -3407,19 +3401,19 @@
         <v>8</v>
       </c>
       <c r="B92" t="s">
+        <v>239</v>
+      </c>
+      <c r="C92" t="s">
+        <v>31</v>
+      </c>
+      <c r="D92" t="s">
+        <v>240</v>
+      </c>
+      <c r="E92" t="s">
         <v>241</v>
       </c>
-      <c r="C92" t="s">
-        <v>32</v>
-      </c>
-      <c r="D92" t="s">
-        <v>242</v>
-      </c>
-      <c r="E92" t="s">
-        <v>243</v>
-      </c>
       <c r="F92" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G92" s="13">
         <v>46060</v>
@@ -3430,19 +3424,19 @@
         <v>8</v>
       </c>
       <c r="B93" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C93" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D93" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E93" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F93" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G93" s="13">
         <v>46060</v>
@@ -3453,19 +3447,19 @@
         <v>8</v>
       </c>
       <c r="B94" t="s">
+        <v>244</v>
+      </c>
+      <c r="C94" t="s">
+        <v>31</v>
+      </c>
+      <c r="D94" t="s">
+        <v>245</v>
+      </c>
+      <c r="E94" t="s">
         <v>246</v>
       </c>
-      <c r="C94" t="s">
-        <v>32</v>
-      </c>
-      <c r="D94" t="s">
-        <v>247</v>
-      </c>
-      <c r="E94" t="s">
-        <v>248</v>
-      </c>
       <c r="F94" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G94" s="13">
         <v>46060</v>
@@ -3476,19 +3470,19 @@
         <v>8</v>
       </c>
       <c r="B95" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C95" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D95" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E95" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F95" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G95" s="13">
         <v>46060</v>
@@ -3499,19 +3493,19 @@
         <v>8</v>
       </c>
       <c r="B96" t="s">
+        <v>249</v>
+      </c>
+      <c r="C96" t="s">
+        <v>31</v>
+      </c>
+      <c r="D96" t="s">
+        <v>250</v>
+      </c>
+      <c r="E96" t="s">
         <v>251</v>
       </c>
-      <c r="C96" t="s">
-        <v>32</v>
-      </c>
-      <c r="D96" t="s">
-        <v>252</v>
-      </c>
-      <c r="E96" t="s">
-        <v>253</v>
-      </c>
       <c r="F96" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G96" s="13">
         <v>46060</v>
@@ -3522,19 +3516,19 @@
         <v>8</v>
       </c>
       <c r="B97" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C97" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D97" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E97" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F97" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G97" s="13">
         <v>46060</v>
@@ -3545,19 +3539,19 @@
         <v>8</v>
       </c>
       <c r="B98" t="s">
+        <v>254</v>
+      </c>
+      <c r="C98" t="s">
+        <v>31</v>
+      </c>
+      <c r="D98" t="s">
+        <v>255</v>
+      </c>
+      <c r="E98" t="s">
         <v>256</v>
       </c>
-      <c r="C98" t="s">
-        <v>32</v>
-      </c>
-      <c r="D98" t="s">
-        <v>257</v>
-      </c>
-      <c r="E98" t="s">
-        <v>258</v>
-      </c>
       <c r="F98" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G98" s="13">
         <v>46060</v>
@@ -3568,19 +3562,19 @@
         <v>8</v>
       </c>
       <c r="B99" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C99" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D99" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E99" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F99" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G99" s="13">
         <v>46060</v>
@@ -3591,19 +3585,19 @@
         <v>8</v>
       </c>
       <c r="B100" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C100" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D100" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E100" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F100" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G100" s="13">
         <v>46060</v>
@@ -3614,19 +3608,19 @@
         <v>8</v>
       </c>
       <c r="B101" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C101" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D101" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E101" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F101" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G101" s="13">
         <v>46060</v>
@@ -3637,19 +3631,19 @@
         <v>8</v>
       </c>
       <c r="B102" t="s">
+        <v>263</v>
+      </c>
+      <c r="C102" t="s">
+        <v>31</v>
+      </c>
+      <c r="D102" t="s">
+        <v>264</v>
+      </c>
+      <c r="E102" t="s">
         <v>265</v>
       </c>
-      <c r="C102" t="s">
-        <v>32</v>
-      </c>
-      <c r="D102" t="s">
-        <v>266</v>
-      </c>
-      <c r="E102" t="s">
-        <v>267</v>
-      </c>
       <c r="F102" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G102" s="13">
         <v>46060</v>
@@ -3660,19 +3654,19 @@
         <v>8</v>
       </c>
       <c r="B103" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C103" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D103" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E103" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F103" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G103" s="13">
         <v>46060</v>
@@ -3683,19 +3677,19 @@
         <v>8</v>
       </c>
       <c r="B104" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C104" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D104" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E104" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F104" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G104" s="13">
         <v>46060</v>

</xml_diff>